<commit_message>
Added A4 + Updated Schematic
</commit_message>
<xml_diff>
--- a/Electronics/BOM.xlsx
+++ b/Electronics/BOM.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Purdue\ECE47700\DodgeBot\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CCAF41-8555-4405-A496-036366721C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6726341-C60F-4CFC-A881-07E7FF5F92C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,15 +38,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
-    <t>STM32F746ZGT6</t>
-  </si>
-  <si>
     <t>LM2678S-5.0/NOPB</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/STM32F746ZGT6/5287179</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/texas-instruments/LM2678S-5.0%2FNOPB/363825?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-363825_sig-CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE</t>
   </si>
   <si>
@@ -126,16 +120,30 @@
   </si>
   <si>
     <t>3.3V Buck Controller</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/STM32F207VGT6TR/4357621</t>
+  </si>
+  <si>
+    <t>STM32F207VGT6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,14 +166,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,7 +511,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,143 +522,154 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>2</v>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>3</v>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>27</v>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
-        <v>5</v>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
-        <v>9</v>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="F8" t="s">
-        <v>18</v>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="F9" t="s">
-        <v>23</v>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{D2248623-79F6-4D46-AA4B-6EF43B761FE0}"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://www.digikey.com/en/products/detail/texas-instruments/LM2678S-5.0%2FNOPB/363825?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-363825_sig-CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiA5L2tBhBTEiwAdSxJX2jmx8jM-JlHhV04F58rlCzi0KZgwJl8jmcjRGNCM7uSaMTsq63izRoCBfYQAvD_BwE" xr:uid="{1931CBDF-70C7-4F6B-9CB6-C2DBEEFCA79F}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{4D664556-4EAB-4E06-A25E-18048DDA20D2}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{72C76521-F886-40B6-9DC9-383265DAAF79}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{1D248C00-639D-482F-831C-6ADD632234C2}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{43827F98-3A79-4A80-B447-26CC33F80E06}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{58686A99-D2B2-4ABB-8E0E-E62B7705CB4F}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{9ECA8115-D7E3-47A9-8A22-A94BE94D64AC}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{423CD540-B29A-4091-92DC-786AE39243E5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Schematic with Main Features
</commit_message>
<xml_diff>
--- a/Electronics/BOM.xlsx
+++ b/Electronics/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Purdue\ECE47700\DodgeBot\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6726341-C60F-4CFC-A881-07E7FF5F92C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AD7851-E489-4C20-A96A-EDF5AA79B5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{B6521EA1-328F-49BB-8E95-1422E8CC3FE5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>LM2678S-5.0/NOPB</t>
   </si>
@@ -86,12 +86,6 @@
     <t>https://www.digikey.com/en/products/detail/vishay-general-semiconductor-diodes-division/VS-6TQ045S-M3/5426222</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/bourns-inc/2300LL-220-V-RC/725902</t>
-  </si>
-  <si>
-    <t>2300LL-220-V-RC</t>
-  </si>
-  <si>
     <t>22uH Inductor</t>
   </si>
   <si>
@@ -126,6 +120,99 @@
   </si>
   <si>
     <t>STM32F207VGT6</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN75ALS174ADWR/1593485</t>
+  </si>
+  <si>
+    <t>SN75ALS174ADWR</t>
+  </si>
+  <si>
+    <t>Line Driver IC</t>
+  </si>
+  <si>
+    <t>SN65LBC175AD</t>
+  </si>
+  <si>
+    <t>Line Receiver IC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN65LBC175AD/380303</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/PJ-202AH/408450</t>
+  </si>
+  <si>
+    <t>PJ-202AH</t>
+  </si>
+  <si>
+    <t>Barrel Jack Connector</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/TPS63700DRCR/1672393</t>
+  </si>
+  <si>
+    <t>Inverting Boost Converter</t>
+  </si>
+  <si>
+    <t>TPS63700DRCR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-general-semiconductor-diodes-division/SL03-GS18/4871689</t>
+  </si>
+  <si>
+    <t>Inv Boost Con. Diode</t>
+  </si>
+  <si>
+    <t>SL03-GS18</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/7443551131/1638545</t>
+  </si>
+  <si>
+    <t>Inv Boost Con. Inductor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/2205-H-RC/775358</t>
+  </si>
+  <si>
+    <t>2300HT-220-H-RC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/3352T-1-203LF/1088346</t>
+  </si>
+  <si>
+    <t>20k Potentiometer</t>
+  </si>
+  <si>
+    <t>3352T-1-203LF</t>
+  </si>
+  <si>
+    <t>General Op-Amp (4 channel)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/OPA4205APWR/17394950</t>
+  </si>
+  <si>
+    <t>OPA4205ADR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/SN75468DR/2255090?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-2255090_sig-CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE</t>
+  </si>
+  <si>
+    <t>NPN Transistor Array</t>
+  </si>
+  <si>
+    <t>SN75468DR</t>
+  </si>
+  <si>
+    <t>ACSL-6400-00TE</t>
+  </si>
+  <si>
+    <t>Optoisolator</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/broadcom-limited/ACSL-6400-00TE/825239</t>
   </si>
 </sst>
 </file>
@@ -508,16 +595,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3747635B-84E0-4BDD-BFA7-D7E59424E192}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -533,7 +620,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -542,7 +629,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -561,16 +648,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -617,44 +704,184 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7443551131</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -668,8 +895,18 @@
     <hyperlink ref="F8" r:id="rId7" xr:uid="{58686A99-D2B2-4ABB-8E0E-E62B7705CB4F}"/>
     <hyperlink ref="F9" r:id="rId8" xr:uid="{9ECA8115-D7E3-47A9-8A22-A94BE94D64AC}"/>
     <hyperlink ref="F10" r:id="rId9" xr:uid="{423CD540-B29A-4091-92DC-786AE39243E5}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{997434B1-B835-4765-875D-6E0D70A7EF79}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{4EE1C4DA-D079-4752-B0F7-C0531C71D7C2}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{00049441-D07F-49F0-97AA-D7EA411D6E00}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{EE0F79CD-B3CB-4D1B-B7CB-1541F6E9176C}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{3CA6F369-FA9F-42AC-A4C2-68BDBB1DC210}"/>
+    <hyperlink ref="F17" r:id="rId15" xr:uid="{E49C395F-D830-4DC4-878B-1F55D58F82B0}"/>
+    <hyperlink ref="F18" r:id="rId16" xr:uid="{42556116-8D5B-4B48-BC82-6B043B471D47}"/>
+    <hyperlink ref="F14" r:id="rId17" xr:uid="{FDDDC4B9-964D-4700-B426-4ED6CF90C007}"/>
+    <hyperlink ref="F19" r:id="rId18" display="https://www.digikey.com/en/products/detail/texas-instruments/SN75468DR/2255090?utm_adgroup=General&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Zombie%20SKUs&amp;utm_term=&amp;utm_content=General&amp;utm_id=go_cmp-17815035045_adg-_ad-__dev-c_ext-_prd-2255090_sig-CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE&amp;gad_source=1&amp;gclid=CjwKCAiAlJKuBhAdEiwAnZb7lY7edhjVnlVUhEyNawogcHzVo6bbfQ1LOtrzO4xh_eCL0cFOX98QUxoCbYMQAvD_BwE" xr:uid="{74361421-FEE6-4D9F-A917-E742AB0C190E}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{58DB788F-9592-4D27-A6F0-2A397ACD43D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>